<commit_message>
hardrive corrupted. some fixes
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C813F564-DC8C-47BE-AE11-49DBB7DAF9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B92AD45-08AF-4942-99C0-A299BBC24A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I52" authorId="1" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
+    <comment ref="I60" authorId="1" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +64,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I63" authorId="2" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
+    <comment ref="I71" authorId="2" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="376">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -1182,6 +1182,30 @@
   </si>
   <si>
     <t>15_02_02_01_two_wheeler_freight</t>
+  </si>
+  <si>
+    <t>15_02_01_05_01_diesel_engine</t>
+  </si>
+  <si>
+    <t>15_02_01_05_02_gasoline_engine</t>
+  </si>
+  <si>
+    <t>15_02_01_05_03_battery_ev</t>
+  </si>
+  <si>
+    <t>15_02_01_05_04_compressed_natual_gas</t>
+  </si>
+  <si>
+    <t>15_02_01_05_05_plugin_hybrid_ev_gasoline</t>
+  </si>
+  <si>
+    <t>15_02_01_05_06_plugin_hybrid_ev_diesel</t>
+  </si>
+  <si>
+    <t>15_02_01_05_07_liquified_petroleum_gas</t>
+  </si>
+  <si>
+    <t>15_02_01_05_08_fuel_cell_ev</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1278,7 +1302,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1603,11 +1626,11 @@
     <text xml:space="preserve">Replaced old values
 </text>
   </threadedComment>
-  <threadedComment ref="I52" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
+  <threadedComment ref="I60" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
     <text xml:space="preserve">Inserted new values
 </text>
   </threadedComment>
-  <threadedComment ref="I63" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
+  <threadedComment ref="I71" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
     <text xml:space="preserve">Inserted new values
 </text>
   </threadedComment>
@@ -1618,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2292,7 +2315,7 @@
         <v>200</v>
       </c>
       <c r="I28" t="s">
-        <v>201</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
@@ -2312,7 +2335,7 @@
         <v>356</v>
       </c>
       <c r="I29" t="s">
-        <v>206</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.35">
@@ -2332,7 +2355,7 @@
         <v>355</v>
       </c>
       <c r="I30" t="s">
-        <v>211</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.35">
@@ -2352,7 +2375,7 @@
         <v>354</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
@@ -2369,7 +2392,7 @@
         <v>357</v>
       </c>
       <c r="I32" t="s">
-        <v>220</v>
+        <v>372</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.35">
@@ -2386,7 +2409,7 @@
         <v>367</v>
       </c>
       <c r="I33" t="s">
-        <v>224</v>
+        <v>373</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.35">
@@ -2403,7 +2426,7 @@
         <v>352</v>
       </c>
       <c r="I34" t="s">
-        <v>228</v>
+        <v>374</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.35">
@@ -2420,7 +2443,7 @@
         <v>353</v>
       </c>
       <c r="I35" t="s">
-        <v>233</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.35">
@@ -2437,7 +2460,7 @@
         <v>232</v>
       </c>
       <c r="I36" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.35">
@@ -2454,7 +2477,7 @@
         <v>237</v>
       </c>
       <c r="I37" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.35">
@@ -2471,7 +2494,7 @@
         <v>242</v>
       </c>
       <c r="I38" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.35">
@@ -2488,7 +2511,7 @@
         <v>247</v>
       </c>
       <c r="I39" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.35">
@@ -2505,7 +2528,7 @@
         <v>252</v>
       </c>
       <c r="I40" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.35">
@@ -2522,7 +2545,7 @@
         <v>257</v>
       </c>
       <c r="I41" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.35">
@@ -2539,7 +2562,7 @@
         <v>262</v>
       </c>
       <c r="I42" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.35">
@@ -2553,7 +2576,7 @@
         <v>266</v>
       </c>
       <c r="I43" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.35">
@@ -2564,7 +2587,7 @@
         <v>269</v>
       </c>
       <c r="I44" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.35">
@@ -2575,7 +2598,7 @@
         <v>272</v>
       </c>
       <c r="I45" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.35">
@@ -2586,7 +2609,7 @@
         <v>275</v>
       </c>
       <c r="I46" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.35">
@@ -2597,7 +2620,7 @@
         <v>278</v>
       </c>
       <c r="I47" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.35">
@@ -2608,7 +2631,7 @@
         <v>281</v>
       </c>
       <c r="I48" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.35">
@@ -2619,7 +2642,7 @@
         <v>284</v>
       </c>
       <c r="I49" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.35">
@@ -2630,7 +2653,7 @@
         <v>287</v>
       </c>
       <c r="I50" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.35">
@@ -2641,7 +2664,7 @@
         <v>290</v>
       </c>
       <c r="I51" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.35">
@@ -2651,188 +2674,210 @@
       <c r="H52" t="s">
         <v>264</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>344</v>
+      <c r="I52" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G53" t="s">
         <v>295</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>345</v>
+      <c r="I53" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G54" t="s">
         <v>296</v>
       </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="5" t="s">
-        <v>346</v>
+      <c r="I54" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G55" t="s">
         <v>297</v>
       </c>
-      <c r="I55" s="5" t="s">
-        <v>347</v>
+      <c r="I55" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G56" t="s">
         <v>298</v>
       </c>
-      <c r="I56" s="5" t="s">
-        <v>348</v>
+      <c r="I56" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G57" t="s">
         <v>299</v>
       </c>
-      <c r="I57" s="5" t="s">
-        <v>349</v>
+      <c r="I57" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G58" t="s">
         <v>300</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>350</v>
+      <c r="I58" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G59" t="s">
         <v>301</v>
       </c>
-      <c r="I59" s="5" t="s">
-        <v>351</v>
+      <c r="I59" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G60" t="s">
         <v>302</v>
       </c>
-      <c r="I60" t="s">
-        <v>264</v>
+      <c r="I60" s="5" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="61" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G61" t="s">
         <v>303</v>
       </c>
+      <c r="I61" s="5" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="62" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G62" t="s">
         <v>304</v>
       </c>
-      <c r="I62" s="8"/>
+      <c r="I62" s="5" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="63" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G63" t="s">
         <v>305</v>
       </c>
-      <c r="I63" s="7" t="s">
-        <v>366</v>
+      <c r="I63" s="5" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="64" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G64" t="s">
         <v>306</v>
       </c>
-      <c r="I64" s="7" t="s">
-        <v>359</v>
+      <c r="I64" s="5" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G65" t="s">
         <v>307</v>
       </c>
-      <c r="I65" s="7" t="s">
-        <v>360</v>
+      <c r="I65" s="5" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="66" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G66" t="s">
         <v>308</v>
       </c>
-      <c r="I66" s="7" t="s">
-        <v>361</v>
+      <c r="I66" s="5" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G67" t="s">
         <v>309</v>
       </c>
-      <c r="I67" s="7" t="s">
-        <v>362</v>
+      <c r="I67" s="5" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G68" t="s">
         <v>310</v>
       </c>
-      <c r="I68" s="7" t="s">
-        <v>363</v>
+      <c r="I68" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G69" t="s">
         <v>311</v>
       </c>
-      <c r="I69" s="7" t="s">
-        <v>364</v>
-      </c>
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G70" t="s">
         <v>312</v>
       </c>
-      <c r="I70" s="7" t="s">
-        <v>365</v>
-      </c>
     </row>
     <row r="71" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G71" t="s">
         <v>313</v>
       </c>
+      <c r="I71" s="7" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="72" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G72" t="s">
         <v>314</v>
       </c>
+      <c r="I72" s="7" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="73" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G73" t="s">
         <v>315</v>
       </c>
+      <c r="I73" s="7" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="74" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G74" t="s">
         <v>316</v>
       </c>
+      <c r="I74" s="7" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="75" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G75" t="s">
         <v>317</v>
       </c>
+      <c r="I75" s="7" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="76" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G76" t="s">
         <v>318</v>
       </c>
+      <c r="I76" s="7" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="77" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G77" t="s">
         <v>319</v>
       </c>
+      <c r="I77" s="7" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="78" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G78" t="s">
         <v>320</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="79" spans="7:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
grouping by 'is_subtotal' in the labeling of subtotals
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B92AD45-08AF-4942-99C0-A299BBC24A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED31C5E-0793-44EC-B7E4-E7011D8942AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'9th_EBT_schema'!$A$3:$I$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,6 +43,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={14F28E3B-E27B-4F10-9E30-A35CE253D9B3}</author>
+    <author>Finbar Barton MAUNSELL</author>
     <author>tc={A9F2DEF1-2471-4600-B89D-8CD286003292}</author>
     <author>tc={27A3B664-367C-45E9-B56B-627DCB291BA1}</author>
   </authors>
@@ -55,7 +57,31 @@
 </t>
       </text>
     </comment>
-    <comment ref="I60" authorId="1" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
+    <comment ref="G48" authorId="1" shapeId="0" xr:uid="{29341040-70C0-4312-AD6B-1FCB698D709B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Finbar Barton MAUNSELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+alex might think about how we could measure own use in ccs. Also need to think about including storage as a own use cateogy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I60" authorId="2" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +90,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I71" authorId="2" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
+    <comment ref="I71" authorId="3" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1212,7 +1238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1235,6 +1261,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1641,29 +1680,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
-    <col min="9" max="9" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1692,7 +1731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1721,7 +1760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1750,7 +1789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -1776,7 +1815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -1802,7 +1841,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -1828,7 +1867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>52</v>
       </c>
@@ -1854,7 +1893,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -1880,7 +1919,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -1906,7 +1945,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>76</v>
       </c>
@@ -1932,7 +1971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>84</v>
       </c>
@@ -1958,7 +1997,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>92</v>
       </c>
@@ -1984,7 +2023,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>100</v>
       </c>
@@ -2010,7 +2049,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>108</v>
       </c>
@@ -2036,7 +2075,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>116</v>
       </c>
@@ -2062,7 +2101,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>124</v>
       </c>
@@ -2088,7 +2127,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -2114,7 +2153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>140</v>
       </c>
@@ -2140,7 +2179,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>148</v>
       </c>
@@ -2166,7 +2205,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>156</v>
       </c>
@@ -2192,7 +2231,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>164</v>
       </c>
@@ -2215,7 +2254,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>171</v>
       </c>
@@ -2238,7 +2277,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>178</v>
       </c>
@@ -2258,7 +2297,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>184</v>
       </c>
@@ -2278,7 +2317,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>190</v>
       </c>
@@ -2298,7 +2337,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>196</v>
       </c>
@@ -2318,7 +2357,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>202</v>
       </c>
@@ -2338,7 +2377,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>207</v>
       </c>
@@ -2358,7 +2397,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>212</v>
       </c>
@@ -2378,7 +2417,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>217</v>
       </c>
@@ -2395,7 +2434,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>221</v>
       </c>
@@ -2412,7 +2451,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>225</v>
       </c>
@@ -2429,7 +2468,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>229</v>
       </c>
@@ -2446,7 +2485,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>234</v>
       </c>
@@ -2463,7 +2502,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>239</v>
       </c>
@@ -2480,7 +2519,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>244</v>
       </c>
@@ -2497,7 +2536,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>249</v>
       </c>
@@ -2514,7 +2553,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>254</v>
       </c>
@@ -2531,7 +2570,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>259</v>
       </c>
@@ -2548,7 +2587,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
         <v>358</v>
       </c>
@@ -2565,7 +2604,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>264</v>
       </c>
@@ -2579,7 +2618,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>271</v>
       </c>
@@ -2590,7 +2629,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>274</v>
       </c>
@@ -2601,7 +2640,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>277</v>
       </c>
@@ -2612,7 +2651,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>280</v>
       </c>
@@ -2623,7 +2662,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>283</v>
       </c>
@@ -2634,7 +2673,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>286</v>
       </c>
@@ -2645,7 +2684,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>289</v>
       </c>
@@ -2656,7 +2695,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>292</v>
       </c>
@@ -2667,7 +2706,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>294</v>
       </c>
@@ -2678,7 +2717,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>295</v>
       </c>
@@ -2686,7 +2725,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>296</v>
       </c>
@@ -2694,7 +2733,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>297</v>
       </c>
@@ -2702,7 +2741,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>298</v>
       </c>
@@ -2710,7 +2749,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
         <v>299</v>
       </c>
@@ -2718,7 +2757,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
         <v>300</v>
       </c>
@@ -2726,7 +2765,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>301</v>
       </c>
@@ -2734,7 +2773,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>302</v>
       </c>
@@ -2742,7 +2781,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>303</v>
       </c>
@@ -2750,7 +2789,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>304</v>
       </c>
@@ -2758,7 +2797,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
         <v>305</v>
       </c>
@@ -2766,7 +2805,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
         <v>306</v>
       </c>
@@ -2774,7 +2813,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
         <v>307</v>
       </c>
@@ -2782,7 +2821,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
         <v>308</v>
       </c>
@@ -2790,7 +2829,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
         <v>309</v>
       </c>
@@ -2798,7 +2837,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
         <v>310</v>
       </c>
@@ -2806,17 +2845,17 @@
         <v>264</v>
       </c>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
         <v>313</v>
       </c>
@@ -2824,7 +2863,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
         <v>314</v>
       </c>
@@ -2832,7 +2871,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
         <v>315</v>
       </c>
@@ -2840,7 +2879,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
         <v>316</v>
       </c>
@@ -2848,7 +2887,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
         <v>317</v>
       </c>
@@ -2856,7 +2895,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
         <v>318</v>
       </c>
@@ -2864,7 +2903,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
         <v>319</v>
       </c>
@@ -2872,7 +2911,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
         <v>320</v>
       </c>
@@ -2880,122 +2919,122 @@
         <v>365</v>
       </c>
     </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
         <v>264</v>
       </c>

</xml_diff>

<commit_message>
update losses and own use subsector labellings
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFDC778-F370-4B1B-833B-0D017ACB7862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19745C73-2B09-4F69-AE09-E6782EFB31BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -777,9 +777,6 @@
     <t>18_electricity_output_in_gwh</t>
   </si>
   <si>
-    <t>10_02_transmision_and_distribution_losses</t>
-  </si>
-  <si>
     <t>09_x_02_gas</t>
   </si>
   <si>
@@ -1104,9 +1101,6 @@
     <t>19_02_heat_plants</t>
   </si>
   <si>
-    <t>10_01_05_natural_gas_blending_plants</t>
-  </si>
-  <si>
     <t>18_01_02_02_combinedcycle</t>
   </si>
   <si>
@@ -1116,102 +1110,66 @@
     <t>x</t>
   </si>
   <si>
-    <t>10_01_08_coke_ovens</t>
-  </si>
-  <si>
     <t>18_01_02_03_ccs</t>
   </si>
   <si>
     <t>15_02_02_03_03_battery_ev</t>
   </si>
   <si>
-    <t>10_01_09_coal_mines</t>
-  </si>
-  <si>
     <t>18_01_05_01_large</t>
   </si>
   <si>
     <t>15_02_02_03_04_compressed_natual_gas</t>
   </si>
   <si>
-    <t>10_01_10_blast_furnaces</t>
-  </si>
-  <si>
     <t>18_01_05_02_mediumsmall</t>
   </si>
   <si>
     <t>15_02_02_03_05_plugin_hybrid_ev_gasoline</t>
   </si>
   <si>
-    <t>10_01_14_oil_refineries</t>
-  </si>
-  <si>
     <t>18_01_05_03_pump</t>
   </si>
   <si>
     <t>15_02_02_03_06_plugin_hybrid_ev_diesel</t>
   </si>
   <si>
-    <t>10_01_15_oil_and_gas_extraction</t>
-  </si>
-  <si>
     <t>18_01_08_01_utility</t>
   </si>
   <si>
     <t>15_02_02_04_01_diesel_engine</t>
   </si>
   <si>
-    <t>10_01_16_biofuels_processing</t>
-  </si>
-  <si>
     <t>18_01_08_02_rooftop</t>
   </si>
   <si>
     <t>15_02_02_04_02_gasoline_engine</t>
   </si>
   <si>
-    <t>10_01_19_ccs</t>
-  </si>
-  <si>
     <t>18_01_08_03_csp</t>
   </si>
   <si>
     <t>15_02_02_04_03_battery_ev</t>
   </si>
   <si>
-    <t>10_01_07_gas_separation</t>
-  </si>
-  <si>
     <t>18_01_09_01_onshore</t>
   </si>
   <si>
     <t>15_02_02_04_04_compressed_natual_gas</t>
   </si>
   <si>
-    <t>10_01_06_gastoliquids_plants</t>
-  </si>
-  <si>
     <t>18_01_09_02_offshore</t>
   </si>
   <si>
     <t>15_02_02_04_05_plugin_hybrid_ev_gasoline</t>
   </si>
   <si>
-    <t>10_01_12_bkb_pb_plants</t>
-  </si>
-  <si>
     <t>15_02_02_04_06_plugin_hybrid_ev_diesel</t>
   </si>
   <si>
-    <t>10_01_18_nonspecified_own_uses</t>
-  </si>
-  <si>
     <t>10_01_02_gas_works_plants</t>
   </si>
   <si>
-    <t>10_01_13_liquefaction_plants_coal_to_oil</t>
-  </si>
-  <si>
     <t>14_03_01_iron_and_steel</t>
   </si>
   <si>
@@ -1447,6 +1405,48 @@
   </si>
   <si>
     <t>15_02_01_05_08_fuel_cell_ev</t>
+  </si>
+  <si>
+    <t>10_01_13_pump_storage_plants</t>
+  </si>
+  <si>
+    <t>10_01_05_coke_ovens</t>
+  </si>
+  <si>
+    <t>10_01_06_coal_mines</t>
+  </si>
+  <si>
+    <t>10_01_07_blast_furnaces</t>
+  </si>
+  <si>
+    <t>10_01_11_oil_refineries</t>
+  </si>
+  <si>
+    <t>10_01_12_oil_and_gas_extraction</t>
+  </si>
+  <si>
+    <t>10_01_15_charcoal_production_plants</t>
+  </si>
+  <si>
+    <t>10_01_18_ccs</t>
+  </si>
+  <si>
+    <t>10_01_16_gasification_plants_for_biogases</t>
+  </si>
+  <si>
+    <t>10_01_04_gastoliquids_plants</t>
+  </si>
+  <si>
+    <t>10_01_09_bkb_pb_plants</t>
+  </si>
+  <si>
+    <t>10_01_17_nonspecified_own_uses</t>
+  </si>
+  <si>
+    <t>10_01_10_liquefaction_plants_coal_to_oil</t>
+  </si>
+  <si>
+    <t>10_02_transmission_and_distribution_losses</t>
   </si>
 </sst>
 </file>
@@ -1931,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,850 +2444,850 @@
         <v>151</v>
       </c>
       <c r="F21" t="s">
+        <v>375</v>
+      </c>
+      <c r="G21" t="s">
         <v>152</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>153</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>154</v>
-      </c>
-      <c r="I21" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>157</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>158</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>159</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>160</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>161</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>162</v>
-      </c>
-      <c r="I22" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" t="s">
         <v>164</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>165</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>166</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>167</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>168</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>169</v>
-      </c>
-      <c r="I23" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" t="s">
         <v>171</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>172</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>173</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>174</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>175</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>176</v>
-      </c>
-      <c r="I24" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" t="s">
         <v>178</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>179</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>180</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>181</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>182</v>
-      </c>
-      <c r="I25" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" t="s">
         <v>184</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>185</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>186</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>187</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>188</v>
-      </c>
-      <c r="I26" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="s">
         <v>190</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>191</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>192</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>193</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>194</v>
-      </c>
-      <c r="I27" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" t="s">
         <v>196</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>197</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>198</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>200</v>
-      </c>
       <c r="I28" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" t="s">
         <v>202</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>203</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>204</v>
       </c>
-      <c r="G29" t="s">
-        <v>205</v>
-      </c>
       <c r="H29" s="6" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="I29" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" t="s">
         <v>207</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>208</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>209</v>
       </c>
-      <c r="G30" t="s">
-        <v>210</v>
-      </c>
       <c r="H30" s="6" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="I30" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
         <v>212</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>213</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>214</v>
       </c>
-      <c r="G31" t="s">
-        <v>215</v>
-      </c>
       <c r="H31" s="6" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="I31" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
         <v>217</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>218</v>
       </c>
-      <c r="G32" t="s">
-        <v>219</v>
-      </c>
       <c r="H32" s="6" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="I32" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
+        <v>220</v>
+      </c>
+      <c r="F33" t="s">
         <v>221</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>222</v>
       </c>
-      <c r="G33" t="s">
-        <v>223</v>
-      </c>
       <c r="H33" s="7" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="I33" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>224</v>
+      </c>
+      <c r="F34" t="s">
         <v>225</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>226</v>
       </c>
-      <c r="G34" t="s">
-        <v>227</v>
-      </c>
       <c r="H34" s="6" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="I34" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35" t="s">
         <v>229</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>230</v>
       </c>
-      <c r="G35" t="s">
-        <v>231</v>
-      </c>
       <c r="H35" s="6" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="I35" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" t="s">
         <v>234</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>235</v>
       </c>
-      <c r="G36" t="s">
-        <v>236</v>
-      </c>
       <c r="H36" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" t="s">
         <v>239</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>240</v>
       </c>
-      <c r="G37" t="s">
-        <v>241</v>
-      </c>
       <c r="H37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" t="s">
         <v>244</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>245</v>
       </c>
-      <c r="G38" t="s">
-        <v>246</v>
-      </c>
       <c r="H38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
+        <v>248</v>
+      </c>
+      <c r="F39" t="s">
         <v>249</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>250</v>
       </c>
-      <c r="G39" t="s">
-        <v>251</v>
-      </c>
       <c r="H39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" t="s">
         <v>254</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>255</v>
       </c>
-      <c r="G40" t="s">
-        <v>256</v>
-      </c>
       <c r="H40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
+        <v>258</v>
+      </c>
+      <c r="F41" t="s">
         <v>259</v>
       </c>
-      <c r="F41" t="s">
-        <v>260</v>
-      </c>
       <c r="G41" t="s">
-        <v>261</v>
+        <v>362</v>
       </c>
       <c r="H41" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="F42" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G42" t="s">
-        <v>265</v>
+        <v>363</v>
       </c>
       <c r="H42" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G43" t="s">
-        <v>268</v>
+        <v>364</v>
       </c>
       <c r="H43" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>271</v>
+        <v>365</v>
       </c>
       <c r="H44" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>274</v>
+        <v>366</v>
       </c>
       <c r="H45" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="I45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>277</v>
+        <v>367</v>
       </c>
       <c r="H46" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>280</v>
+        <v>368</v>
       </c>
       <c r="H47" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="I47" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>283</v>
+        <v>369</v>
       </c>
       <c r="H48" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="I48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>286</v>
+        <v>370</v>
       </c>
       <c r="H49" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="I49" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="H50" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="I50" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>292</v>
+        <v>372</v>
       </c>
       <c r="H51" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="I51" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>294</v>
+        <v>373</v>
       </c>
       <c r="H52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I52" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="I53" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>296</v>
+        <v>374</v>
       </c>
       <c r="I54" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="I55" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="I56" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="I57" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="I58" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="I59" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="66" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="I68" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="73" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="75" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 19_02_05_others and 19_02_17_electricity in config
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19745C73-2B09-4F69-AE09-E6782EFB31BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018010F8-CF74-4969-9570-3426D5C17D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="379">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -1447,6 +1447,15 @@
   </si>
   <si>
     <t>10_02_transmission_and_distribution_losses</t>
+  </si>
+  <si>
+    <t>19_02_05_others</t>
+  </si>
+  <si>
+    <t>19_02_17_electricity</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1616,9 +1625,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1656,7 +1665,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1762,7 +1771,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1904,7 +1913,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1929,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,7 +3296,17 @@
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>262</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addded new sub2sectors 18_01_02_gas_power_ccs
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018010F8-CF74-4969-9570-3426D5C17D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47651AB1-2791-4C4A-BC41-A72D7A0E6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'9th_EBT_schema'!$A$3:$I$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'9th_EBT_schema'!$A$3:$I$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -151,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -160,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not an ouput from power</t>
@@ -175,7 +175,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -184,7 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 should add 05_other</t>
@@ -199,7 +199,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -208,7 +208,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 relatively useless</t>
@@ -223,7 +223,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -232,7 +232,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 relatively useless</t>
@@ -247,7 +247,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -256,7 +256,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 we should add 9_x_others, 9_X_elec and probably more</t>
@@ -272,7 +272,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="G48" authorId="0" shapeId="0" xr:uid="{29341040-70C0-4312-AD6B-1FCB698D709B}">
+    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{29341040-70C0-4312-AD6B-1FCB698D709B}">
       <text>
         <r>
           <rPr>
@@ -280,7 +280,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Finbar Barton MAUNSELL:</t>
         </r>
@@ -289,14 +289,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 alex might think about how we could measure own use in ccs. Also need to think about including storage as a own use cateogy</t>
         </r>
       </text>
     </comment>
-    <comment ref="I60" authorId="2" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
+    <comment ref="I57" authorId="2" shapeId="0" xr:uid="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -305,7 +305,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I71" authorId="3" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
+    <comment ref="I68" authorId="3" shapeId="0" xr:uid="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="367">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -990,9 +990,6 @@
     <t>09_13_01_electrolysers</t>
   </si>
   <si>
-    <t>15_02_02_01_06_plugin_hybrid_ev_diesel</t>
-  </si>
-  <si>
     <t>16_04_municipal_solid_waste_nonrenewable</t>
   </si>
   <si>
@@ -1002,9 +999,6 @@
     <t>09_13_02_smr_wo_ccs</t>
   </si>
   <si>
-    <t>15_02_02_02_01_diesel_engine</t>
-  </si>
-  <si>
     <t>16_05_biogasoline</t>
   </si>
   <si>
@@ -1017,9 +1011,6 @@
     <t>15_02_02_04_heavy_truck</t>
   </si>
   <si>
-    <t>15_02_02_02_02_gasoline_engine</t>
-  </si>
-  <si>
     <t>16_06_biodiesel</t>
   </si>
   <si>
@@ -1089,30 +1080,15 @@
     <t>10_01_03_liquefaction_regasification_plants</t>
   </si>
   <si>
-    <t>18_01_02_01_gasturbine</t>
-  </si>
-  <si>
     <t>15_02_02_03_01_diesel_engine</t>
   </si>
   <si>
-    <t>16_x_hydrogen</t>
-  </si>
-  <si>
-    <t>19_02_heat_plants</t>
-  </si>
-  <si>
-    <t>18_01_02_02_combinedcycle</t>
-  </si>
-  <si>
     <t>15_02_02_03_02_gasoline_engine</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>18_01_02_03_ccs</t>
-  </si>
-  <si>
     <t>15_02_02_03_03_battery_ev</t>
   </si>
   <si>
@@ -1353,9 +1329,6 @@
     <t>15_02_01_05_bus</t>
   </si>
   <si>
-    <t>16_x_efuel</t>
-  </si>
-  <si>
     <t>15_02_01_02_08_fuel_cell_ev</t>
   </si>
   <si>
@@ -1407,15 +1380,6 @@
     <t>15_02_01_05_08_fuel_cell_ev</t>
   </si>
   <si>
-    <t>10_01_13_pump_storage_plants</t>
-  </si>
-  <si>
-    <t>10_01_05_coke_ovens</t>
-  </si>
-  <si>
-    <t>10_01_06_coal_mines</t>
-  </si>
-  <si>
     <t>10_01_07_blast_furnaces</t>
   </si>
   <si>
@@ -1455,14 +1419,14 @@
     <t>19_02_17_electricity</t>
   </si>
   <si>
-    <t>s</t>
+    <t>18_01_02_gas_power_ccs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1490,26 +1454,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1518,6 +1462,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1600,7 +1551,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1925,11 +1876,11 @@
     <text xml:space="preserve">Replaced old values
 </text>
   </threadedComment>
-  <threadedComment ref="I60" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
+  <threadedComment ref="I57" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{A9F2DEF1-2471-4600-B89D-8CD286003292}">
     <text xml:space="preserve">Inserted new values
 </text>
   </threadedComment>
-  <threadedComment ref="I71" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
+  <threadedComment ref="I68" dT="2023-07-11T01:57:02.86" personId="{BA1659A9-4D52-4F46-B8E6-CECE8A23AF6D}" id="{27A3B664-367C-45E9-B56B-627DCB291BA1}">
     <text xml:space="preserve">Inserted new values
 </text>
   </threadedComment>
@@ -1938,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2404,7 @@
         <v>151</v>
       </c>
       <c r="F21" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G21" t="s">
         <v>152</v>
@@ -2614,7 +2565,7 @@
         <v>199</v>
       </c>
       <c r="I28" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -2631,10 +2582,10 @@
         <v>204</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I29" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -2651,10 +2602,10 @@
         <v>209</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="I30" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -2671,10 +2622,10 @@
         <v>214</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="I31" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -2688,10 +2639,10 @@
         <v>218</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="I32" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
@@ -2705,58 +2656,58 @@
         <v>222</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="I33" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>223</v>
+      </c>
+      <c r="F34" t="s">
         <v>224</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>225</v>
       </c>
-      <c r="G34" t="s">
-        <v>226</v>
-      </c>
       <c r="H34" s="6" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="I34" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
+        <v>226</v>
+      </c>
+      <c r="F35" t="s">
+        <v>227</v>
+      </c>
+      <c r="G35" t="s">
         <v>228</v>
       </c>
-      <c r="F35" t="s">
-        <v>229</v>
-      </c>
-      <c r="G35" t="s">
-        <v>230</v>
-      </c>
       <c r="H35" s="6" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="I35" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F36" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G36" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I36" t="s">
         <v>200</v>
@@ -2764,16 +2715,16 @@
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G37" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I37" t="s">
         <v>205</v>
@@ -2781,16 +2732,16 @@
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F38" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G38" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H38" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I38" t="s">
         <v>210</v>
@@ -2798,16 +2749,16 @@
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G39" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H39" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I39" t="s">
         <v>215</v>
@@ -2815,502 +2766,459 @@
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F40" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G40" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H40" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I40" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>258</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
+        <v>353</v>
+      </c>
+      <c r="H41" t="s">
+        <v>257</v>
+      </c>
+      <c r="I41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>354</v>
+      </c>
+      <c r="H42" t="s">
         <v>259</v>
       </c>
-      <c r="G41" t="s">
-        <v>362</v>
-      </c>
-      <c r="H41" t="s">
-        <v>256</v>
-      </c>
-      <c r="I41" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="F42" t="s">
-        <v>262</v>
-      </c>
-      <c r="G42" t="s">
-        <v>363</v>
-      </c>
-      <c r="H42" t="s">
-        <v>260</v>
-      </c>
       <c r="I42" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>262</v>
-      </c>
       <c r="G43" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="H43" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I43" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="H44" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I44" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="H45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I45" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="H46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I46" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="H47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I47" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="H48" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I48" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="H49" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="I49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>371</v>
-      </c>
-      <c r="H50" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I50" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>372</v>
-      </c>
-      <c r="H51" t="s">
-        <v>279</v>
+        <v>362</v>
       </c>
       <c r="I51" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>373</v>
-      </c>
-      <c r="H52" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="I52" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="I53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>374</v>
+        <v>277</v>
       </c>
       <c r="I54" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I56" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>285</v>
-      </c>
-      <c r="I57" t="s">
-        <v>278</v>
+        <v>280</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>286</v>
-      </c>
-      <c r="I58" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>287</v>
-      </c>
-      <c r="I59" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>293</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>335</v>
+        <v>288</v>
+      </c>
+      <c r="I65" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="66" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>294</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>336</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>295</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>337</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>296</v>
-      </c>
-      <c r="I68" t="s">
-        <v>262</v>
+        <v>291</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="69" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
-        <v>297</v>
+        <v>292</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="74" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="75" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
-        <v>304</v>
-      </c>
-      <c r="I76" s="7" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
-        <v>305</v>
-      </c>
-      <c r="I77" s="7" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="78" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>306</v>
-      </c>
-      <c r="I78" s="7" t="s">
-        <v>351</v>
+        <v>300</v>
       </c>
     </row>
     <row r="79" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="80" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>328</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
-        <v>329</v>
+        <v>365</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G103" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G104" t="s">
-        <v>378</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:I102" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}"/>
+  <autoFilter ref="A3:I99" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
lots of little things.
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD0AA42-5A11-45A5-A853-E7C518E795E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB19EFB-F915-4457-8878-C60A3A0E6748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22050" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -1426,6 +1426,12 @@
   </si>
   <si>
     <t>09_01_02_gas_power_ccs</t>
+  </si>
+  <si>
+    <t>16_01_03_ai_training</t>
+  </si>
+  <si>
+    <t>16_01_04_traditional_data_centres</t>
   </si>
 </sst>
 </file>
@@ -1895,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3231,6 +3237,16 @@
         <v>255</v>
       </c>
     </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:I99" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates to handle data centres
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65047C36-FA70-4308-AFDB-8AE2EBC63DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE1973D-5E8F-40CC-815E-2D5F5691B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -1428,10 +1428,10 @@
     <t>09_01_02_gas_power_ccs</t>
   </si>
   <si>
-    <t>16_01_03_traditional_data_centres</t>
-  </si>
-  <si>
-    <t>16_01_04_ai_training</t>
+    <t>16_01_04_traditional_data_centres</t>
+  </si>
+  <si>
+    <t>16_01_03_ai_training</t>
   </si>
 </sst>
 </file>
@@ -1903,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G75" sqref="G74:G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implemented method for unallocated subfuels
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB19EFB-F915-4457-8878-C60A3A0E6748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6C7EE-B2FF-41AC-A32E-B13EFA17DC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="375">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -1432,6 +1432,18 @@
   </si>
   <si>
     <t>16_01_04_traditional_data_centres</t>
+  </si>
+  <si>
+    <t>16_x_hydrogen</t>
+  </si>
+  <si>
+    <t>16_x_efuel</t>
+  </si>
+  <si>
+    <t>16_others_unallocated</t>
+  </si>
+  <si>
+    <t>15_solid_biomass_unallocated</t>
   </si>
 </sst>
 </file>
@@ -1579,6 +1591,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1411941</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0447F309-36B9-78A6-4CC5-4337BE8F92EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3709147" y="1322294"/>
+          <a:ext cx="6107206" cy="3070412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>dont think this is up to date</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> for sectors - 2/12/2025</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1903,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,6 +2889,9 @@
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>371</v>
+      </c>
       <c r="G41" t="s">
         <v>252</v>
       </c>
@@ -2808,6 +2903,9 @@
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>372</v>
+      </c>
       <c r="G42" t="s">
         <v>353</v>
       </c>
@@ -2819,6 +2917,9 @@
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>373</v>
+      </c>
       <c r="G43" t="s">
         <v>354</v>
       </c>
@@ -2830,6 +2931,9 @@
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>374</v>
+      </c>
       <c r="G44" t="s">
         <v>355</v>
       </c>
@@ -3251,6 +3355,7 @@
   <autoFilter ref="A3:I99" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new agri files and 18_CT bad values in production
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB19EFB-F915-4457-8878-C60A3A0E6748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEC1805-F649-4E23-8BAE-97C72FCEBFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -167,30 +167,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{BB7B3B9B-6B4E-472A-BC71-8146B43887F2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Finbar Barton MAUNSELL:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-should add 05_other</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E21" authorId="0" shapeId="0" xr:uid="{399AAAA4-A2D3-456E-B9A5-F6BF06B2AA44}">
       <text>
         <r>
@@ -212,6 +188,30 @@
           </rPr>
           <t xml:space="preserve">
 relatively useless</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{BB7B3B9B-6B4E-472A-BC71-8146B43887F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Finbar Barton MAUNSELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+should add 05_other</t>
         </r>
       </text>
     </comment>
@@ -239,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{D23D7952-542C-4A40-BE82-6833AB082B35}">
+    <comment ref="G25" authorId="0" shapeId="0" xr:uid="{D23D7952-542C-4A40-BE82-6833AB082B35}">
       <text>
         <r>
           <rPr>
@@ -272,7 +272,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="G46" authorId="0" shapeId="0" xr:uid="{29341040-70C0-4312-AD6B-1FCB698D709B}">
+    <comment ref="G47" authorId="0" shapeId="0" xr:uid="{29341040-70C0-4312-AD6B-1FCB698D709B}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="373">
   <si>
     <t>Variables (fuels and sectors 'lined-up' in subsequent sheets)</t>
   </si>
@@ -1432,6 +1432,12 @@
   </si>
   <si>
     <t>16_01_04_traditional_data_centres</t>
+  </si>
+  <si>
+    <t>09_01_02_gas_power_h2</t>
+  </si>
+  <si>
+    <t>18_01_02_gas_power_h2</t>
   </si>
 </sst>
 </file>
@@ -1901,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2061,7 @@
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>371</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>42</v>
@@ -2081,7 +2087,7 @@
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>50</v>
@@ -2107,7 +2113,7 @@
         <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>58</v>
@@ -2133,7 +2139,7 @@
         <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>66</v>
@@ -2159,7 +2165,7 @@
         <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>74</v>
@@ -2185,7 +2191,7 @@
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>82</v>
@@ -2211,7 +2217,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>90</v>
@@ -2237,7 +2243,7 @@
         <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
         <v>98</v>
@@ -2263,7 +2269,7 @@
         <v>104</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
         <v>106</v>
@@ -2289,7 +2295,7 @@
         <v>112</v>
       </c>
       <c r="G16" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
         <v>114</v>
@@ -2315,7 +2321,7 @@
         <v>120</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H17" t="s">
         <v>122</v>
@@ -2341,7 +2347,7 @@
         <v>128</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
         <v>130</v>
@@ -2367,7 +2373,7 @@
         <v>136</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
         <v>138</v>
@@ -2393,7 +2399,7 @@
         <v>144</v>
       </c>
       <c r="G20" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H20" t="s">
         <v>146</v>
@@ -2419,7 +2425,7 @@
         <v>363</v>
       </c>
       <c r="G21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H21" t="s">
         <v>153</v>
@@ -2445,7 +2451,7 @@
         <v>159</v>
       </c>
       <c r="G22" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H22" t="s">
         <v>161</v>
@@ -2468,7 +2474,7 @@
         <v>166</v>
       </c>
       <c r="G23" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H23" t="s">
         <v>168</v>
@@ -2491,7 +2497,7 @@
         <v>173</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H24" t="s">
         <v>175</v>
@@ -2514,7 +2520,7 @@
         <v>179</v>
       </c>
       <c r="G25" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H25" t="s">
         <v>181</v>
@@ -2534,7 +2540,7 @@
         <v>185</v>
       </c>
       <c r="G26" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H26" t="s">
         <v>187</v>
@@ -2554,7 +2560,7 @@
         <v>191</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H27" t="s">
         <v>193</v>
@@ -2574,7 +2580,7 @@
         <v>197</v>
       </c>
       <c r="G28" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>199</v>
@@ -2594,7 +2600,7 @@
         <v>203</v>
       </c>
       <c r="G29" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>334</v>
@@ -2614,7 +2620,7 @@
         <v>208</v>
       </c>
       <c r="G30" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>333</v>
@@ -2634,7 +2640,7 @@
         <v>213</v>
       </c>
       <c r="G31" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>332</v>
@@ -2651,7 +2657,7 @@
         <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>335</v>
@@ -2668,7 +2674,7 @@
         <v>221</v>
       </c>
       <c r="G33" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>344</v>
@@ -2685,7 +2691,7 @@
         <v>224</v>
       </c>
       <c r="G34" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>330</v>
@@ -2702,7 +2708,7 @@
         <v>227</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>331</v>
@@ -2719,7 +2725,7 @@
         <v>231</v>
       </c>
       <c r="G36" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>229</v>
@@ -2736,7 +2742,7 @@
         <v>236</v>
       </c>
       <c r="G37" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H37" t="s">
         <v>233</v>
@@ -2753,7 +2759,7 @@
         <v>241</v>
       </c>
       <c r="G38" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H38" t="s">
         <v>238</v>
@@ -2770,7 +2776,7 @@
         <v>246</v>
       </c>
       <c r="G39" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H39" t="s">
         <v>243</v>
@@ -2787,7 +2793,7 @@
         <v>251</v>
       </c>
       <c r="G40" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H40" t="s">
         <v>248</v>
@@ -2798,7 +2804,7 @@
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H41" t="s">
         <v>257</v>
@@ -2809,7 +2815,7 @@
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>353</v>
+        <v>252</v>
       </c>
       <c r="H42" t="s">
         <v>259</v>
@@ -2820,7 +2826,7 @@
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H43" t="s">
         <v>261</v>
@@ -2831,7 +2837,7 @@
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H44" t="s">
         <v>263</v>
@@ -2842,7 +2848,7 @@
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H45" t="s">
         <v>265</v>
@@ -2853,7 +2859,7 @@
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H46" t="s">
         <v>267</v>
@@ -2864,7 +2870,7 @@
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H47" t="s">
         <v>269</v>
@@ -2875,7 +2881,7 @@
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H48" t="s">
         <v>271</v>
@@ -2886,7 +2892,7 @@
     </row>
     <row r="49" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" t="s">
         <v>255</v>
@@ -2897,7 +2903,7 @@
     </row>
     <row r="50" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I50" t="s">
         <v>262</v>
@@ -2905,7 +2911,7 @@
     </row>
     <row r="51" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>274</v>
+        <v>361</v>
       </c>
       <c r="I51" t="s">
         <v>264</v>
@@ -2913,7 +2919,7 @@
     </row>
     <row r="52" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>362</v>
+        <v>274</v>
       </c>
       <c r="I52" t="s">
         <v>266</v>
@@ -2921,7 +2927,7 @@
     </row>
     <row r="53" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>275</v>
+        <v>362</v>
       </c>
       <c r="I53" t="s">
         <v>268</v>
@@ -2929,7 +2935,7 @@
     </row>
     <row r="54" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I54" t="s">
         <v>270</v>
@@ -2937,7 +2943,7 @@
     </row>
     <row r="55" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I55" t="s">
         <v>272</v>
@@ -2945,7 +2951,7 @@
     </row>
     <row r="56" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I56" t="s">
         <v>273</v>
@@ -2953,7 +2959,7 @@
     </row>
     <row r="57" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>322</v>
@@ -2961,7 +2967,7 @@
     </row>
     <row r="58" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>323</v>
@@ -2969,7 +2975,7 @@
     </row>
     <row r="59" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>324</v>
@@ -2977,7 +2983,7 @@
     </row>
     <row r="60" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>325</v>
@@ -2985,7 +2991,7 @@
     </row>
     <row r="61" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>326</v>
@@ -2993,7 +2999,7 @@
     </row>
     <row r="62" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>327</v>
@@ -3001,7 +3007,7 @@
     </row>
     <row r="63" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>328</v>
@@ -3009,7 +3015,7 @@
     </row>
     <row r="64" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>329</v>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="65" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I65" t="s">
         <v>255</v>
@@ -3025,17 +3031,17 @@
     </row>
     <row r="66" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="67" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="68" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>343</v>
@@ -3043,7 +3049,7 @@
     </row>
     <row r="69" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>336</v>
@@ -3051,7 +3057,7 @@
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>337</v>
@@ -3059,7 +3065,7 @@
     </row>
     <row r="71" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I71" s="7" t="s">
         <v>338</v>
@@ -3067,7 +3073,7 @@
     </row>
     <row r="72" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>339</v>
@@ -3075,7 +3081,7 @@
     </row>
     <row r="73" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>340</v>
@@ -3083,7 +3089,7 @@
     </row>
     <row r="74" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>341</v>
@@ -3091,7 +3097,7 @@
     </row>
     <row r="75" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>342</v>
@@ -3099,151 +3105,161 @@
     </row>
     <row r="76" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="77" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
     </row>
     <row r="79" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>300</v>
+        <v>366</v>
       </c>
     </row>
     <row r="80" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
-        <v>301</v>
+        <v>372</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
     </row>
     <row r="103" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G103" t="s">
-        <v>255</v>
+        <v>364</v>
       </c>
     </row>
     <row r="104" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G104" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="105" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G105" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
         <v>370</v>
       </c>
     </row>

</xml_diff>